<commit_message>
feat(files): Agregado version actualizada del extracto bancario
</commit_message>
<xml_diff>
--- a/public/files/example_extract_bank.xlsx
+++ b/public/files/example_extract_bank.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Fecha</t>
   </si>
@@ -28,6 +28,18 @@
     <t>HOJA DE RUTA</t>
   </si>
   <si>
+    <t>PAGADO POR (RECOJO DE DOCUMENTOS)</t>
+  </si>
+  <si>
+    <t>MÉTODOS DE PAGO DE RECOJO/RECEPCIÓN</t>
+  </si>
+  <si>
+    <t>CONFIRMACIÓN DE MONTO PAGADO POR RECOJO/RECEPCIÓN (BS)</t>
+  </si>
+  <si>
+    <t>*GERENCIA* ESTADO DE PAGO (RECOJO DE DCTOS)</t>
+  </si>
+  <si>
     <t>-14,602.00</t>
   </si>
   <si>
@@ -37,6 +49,9 @@
     <t>2024-0309</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>-454.90</t>
   </si>
   <si>
@@ -56,9 +71,6 @@
   </si>
   <si>
     <t>21,000.00</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>2024-0344</t>
@@ -74,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -83,12 +95,8 @@
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="11.0"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -100,11 +108,20 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,32 +130,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5B9BD5"/>
-        <bgColor rgb="FF5B9BD5"/>
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEA4335"/>
-        <bgColor rgb="FFEA4335"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor rgb="FFDDEBF7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -167,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -177,50 +176,47 @@
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -444,8 +440,11 @@
     <col customWidth="1" min="2" max="2" width="19.0"/>
     <col customWidth="1" min="3" max="3" width="17.25"/>
     <col customWidth="1" min="4" max="4" width="19.5"/>
-    <col customWidth="1" min="8" max="8" width="21.63"/>
-    <col customWidth="1" min="9" max="9" width="15.75"/>
+    <col customWidth="1" min="5" max="5" width="13.5"/>
+    <col customWidth="1" min="6" max="6" width="42.88"/>
+    <col customWidth="1" min="7" max="7" width="45.25"/>
+    <col customWidth="1" min="8" max="8" width="67.75"/>
+    <col customWidth="1" min="9" max="9" width="52.25"/>
     <col customWidth="1" min="12" max="12" width="17.63"/>
   </cols>
   <sheetData>
@@ -465,157 +464,231 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>45418.0</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>2141702.0</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>45418.0</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>3.781715945E9</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>45418.0</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>2141764.0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
+      <c r="E4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <v>45418.0</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>3.781745419E9</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>45418.0</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>3.781747287E9</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="C6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9">
+        <v>45418.0</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3.781748202E9</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="11">
-        <v>45418.0</v>
-      </c>
-      <c r="B7" s="12">
-        <v>3.781748202E9</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="F7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
     </row>
     <row r="19">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
feat(banks): Actualiza la plantilla del extracto bancario
</commit_message>
<xml_diff>
--- a/public/files/example_extract_bank.xlsx
+++ b/public/files/example_extract_bank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23730" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -27,15 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Fecha</t>
+    <t>FECHA</t>
   </si>
   <si>
-    <t>Nro Documento</t>
+    <t>NRO DOCUMENTO</t>
   </si>
   <si>
-    <t>Monto</t>
+    <t>MONTO</t>
   </si>
   <si>
     <t>GLOSA EN EXTRACTO</t>
@@ -55,15 +55,6 @@
   <si>
     <t>VALOR DE PAGO</t>
   </si>
-  <si>
-    <t>ANB</t>
-  </si>
-  <si>
-    <t>2024-0829</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
 </sst>
 </file>
 
@@ -76,7 +67,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -86,17 +77,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -286,15 +270,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,12 +288,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.4"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -522,9 +493,7 @@
       <top style="thin">
         <color rgb="FF9BC2E6"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF9BC2E6"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -533,9 +502,7 @@
       <top style="thin">
         <color rgb="FF9BC2E6"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF9BC2E6"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -648,67 +615,70 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -723,78 +693,75 @@
     <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -803,39 +770,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,17 +1301,17 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="17.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="19.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="13.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="42.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="23.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="15.2666666666667" customWidth="1"/>
+    <col min="6" max="6" width="49.5714285714286" customWidth="1"/>
     <col min="7" max="7" width="45.2857142857143" customWidth="1"/>
     <col min="8" max="8" width="67.7142857142857" customWidth="1"/>
     <col min="9" max="9" width="52.2857142857143" customWidth="1"/>
@@ -1360,153 +1347,133 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" customHeight="1" spans="1:12">
-      <c r="A2" s="5">
-        <v>45418</v>
-      </c>
-      <c r="B2" s="6">
-        <v>2141702</v>
-      </c>
-      <c r="C2" s="7">
-        <v>14602</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="15"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" customHeight="1" spans="1:12">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="15"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" customHeight="1" spans="1:12">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="23"/>
     </row>
     <row r="5" customHeight="1" spans="1:12">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" customHeight="1" spans="1:12">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" customHeight="1" spans="1:9">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+    <row r="8" customHeight="1" spans="1:6">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
     </row>
-    <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+    <row r="9" customHeight="1" spans="1:6">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" customHeight="1" spans="4:6">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" customHeight="1" spans="4:6">
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" customHeight="1" spans="4:6">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" customHeight="1" spans="4:6">
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(banks): Actualizar la plantilla de extracto bancario
</commit_message>
<xml_diff>
--- a/public/files/example_extract_bank.xlsx
+++ b/public/files/example_extract_bank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12885"/>
+    <workbookView windowWidth="20175" windowHeight="9615"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>FECHA</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>GLOSA EN EXTRACTO</t>
+  </si>
+  <si>
+    <t>CODIGO CONTRA CUENTA</t>
+  </si>
+  <si>
+    <t>TIPO DE TRANSACCION</t>
   </si>
   <si>
     <t>HOJA DE RUTA</t>
@@ -55,6 +61,9 @@
   <si>
     <t>VALOR DE PAGO</t>
   </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
@@ -280,13 +289,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +770,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,6 +778,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -779,19 +791,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,9 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1299,10 +1299,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5714285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -1310,16 +1310,17 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="17.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="23.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="15.2666666666667" customWidth="1"/>
-    <col min="6" max="6" width="49.5714285714286" customWidth="1"/>
-    <col min="7" max="7" width="45.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="67.7142857142857" customWidth="1"/>
-    <col min="9" max="9" width="52.2857142857143" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="12" max="12" width="17.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="28.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="24.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="49.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="45.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="67.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="52.2857142857143" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
+    <col min="13" max="13" width="17.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:12">
+    <row r="1" customHeight="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1335,145 +1336,186 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="20"/>
     </row>
-    <row r="2" customHeight="1" spans="1:12">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="23"/>
+    <row r="2" customHeight="1" spans="1:13">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="19"/>
+      <c r="M2" s="20"/>
     </row>
-    <row r="3" customHeight="1" spans="1:12">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
+    <row r="3" customHeight="1" spans="1:13">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
     </row>
-    <row r="4" customHeight="1" spans="1:12">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+    <row r="4" customHeight="1" spans="1:13">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="20"/>
     </row>
-    <row r="5" customHeight="1" spans="1:12">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+    <row r="5" customHeight="1" spans="1:13">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="23"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
     </row>
-    <row r="6" customHeight="1" spans="1:12">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="9"/>
+    <row r="6" customHeight="1" spans="1:13">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="23"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
     </row>
-    <row r="7" customHeight="1" spans="1:9">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="9"/>
+    <row r="7" customHeight="1" spans="1:10">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
-    <row r="8" customHeight="1" spans="1:6">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+    <row r="8" customHeight="1" spans="1:7">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
     </row>
-    <row r="9" customHeight="1" spans="1:6">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="18"/>
+    <row r="9" customHeight="1" spans="1:7">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
     </row>
-    <row r="10" customHeight="1" spans="4:6">
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+    <row r="10" customHeight="1" spans="4:7">
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
-    <row r="11" customHeight="1" spans="4:6">
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+    <row r="11" customHeight="1" spans="4:7">
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
     </row>
-    <row r="12" customHeight="1" spans="4:6">
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
+    <row r="12" customHeight="1" spans="4:7">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
-    <row r="13" customHeight="1" spans="4:6">
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+    <row r="13" customHeight="1" spans="4:7">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
-    <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+    <row r="19" customHeight="1" spans="1:6">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>